<commit_message>
Added feature to check if cell is already hyperlinked, added both windows file path and linux file path.
</commit_message>
<xml_diff>
--- a/workbooks/Change Log.xlsx
+++ b/workbooks/Change Log.xlsx
@@ -215,13 +215,13 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.3"/>
@@ -248,7 +248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added new test files, and update getSplitMessage method to handle messages titled with hyphens and no spaces.
</commit_message>
<xml_diff>
--- a/workbooks/Change Log.xlsx
+++ b/workbooks/Change Log.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t xml:space="preserve">Customer Name</t>
   </si>
@@ -101,6 +101,24 @@
   </si>
   <si>
     <t xml:space="preserve">Stuff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walmart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJH098987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">things</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPJD000061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
   </si>
 </sst>
 </file>
@@ -212,13 +230,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.04"/>
@@ -435,6 +453,40 @@
         <v>9</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>